<commit_message>
Changed the way everything is printned in the connsole because of an error in the way SampleTable was formatted. This should now be fixed.
</commit_message>
<xml_diff>
--- a/sampleTable.xlsx
+++ b/sampleTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lennc\Desktop\S5\Z-Z-GitHub\pythonShenanigens\python_excel_read_write\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528679A8-80DD-48E9-B4A1-816C0E28655D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73F6838-BC0E-4DF4-9C94-BE92FD4DC32F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,10 +70,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,176 +353,173 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A2:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1">
-        <v>33.130000000000003</v>
-      </c>
-      <c r="B1" s="1">
-        <v>32.979999999999997</v>
-      </c>
-      <c r="C1" s="1">
-        <v>36.51</v>
-      </c>
-      <c r="D1" s="1">
-        <v>33.65</v>
-      </c>
-      <c r="E1" s="1">
-        <v>33.65</v>
-      </c>
-      <c r="F1" s="1">
-        <v>37.01</v>
-      </c>
-      <c r="G1" s="1">
-        <v>33.79</v>
-      </c>
-      <c r="H1" s="1">
-        <v>34.81</v>
-      </c>
-      <c r="I1" s="1">
-        <v>40.22</v>
-      </c>
-    </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>33.799999999999997</v>
+        <v>33.130000000000003</v>
       </c>
       <c r="B2" s="1">
-        <v>33.61</v>
+        <v>32.979999999999997</v>
       </c>
       <c r="C2" s="1">
-        <v>36.04</v>
+        <v>36.51</v>
       </c>
       <c r="D2" s="1">
-        <v>33.47</v>
+        <v>33.65</v>
       </c>
       <c r="E2" s="1">
-        <v>34.479999999999997</v>
+        <v>33.65</v>
       </c>
       <c r="F2" s="1">
-        <v>36.43</v>
+        <v>37.01</v>
       </c>
       <c r="G2" s="1">
-        <v>34.770000000000003</v>
+        <v>33.79</v>
       </c>
       <c r="H2" s="1">
         <v>34.81</v>
       </c>
       <c r="I2" s="1">
-        <v>39.57</v>
+        <v>40.22</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>35.58</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="B3" s="1">
-        <v>35.799999999999997</v>
+        <v>33.61</v>
       </c>
       <c r="C3" s="1">
-        <v>39.51</v>
+        <v>36.04</v>
       </c>
       <c r="D3" s="1">
-        <v>35.159999999999997</v>
+        <v>33.47</v>
       </c>
       <c r="E3" s="1">
-        <v>36.299999999999997</v>
+        <v>34.479999999999997</v>
       </c>
       <c r="F3" s="1">
-        <v>39.94</v>
+        <v>36.43</v>
       </c>
       <c r="G3" s="1">
-        <v>36.4</v>
+        <v>34.770000000000003</v>
       </c>
       <c r="H3" s="1">
-        <v>37.31</v>
+        <v>34.81</v>
       </c>
       <c r="I3" s="1">
-        <v>43.03</v>
+        <v>39.57</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>35.58</v>
+      </c>
       <c r="B4" s="1">
-        <v>35.950000000000003</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="C4" s="1">
-        <v>39.36</v>
+        <v>39.51</v>
       </c>
       <c r="D4" s="1">
-        <v>35.22</v>
+        <v>35.159999999999997</v>
       </c>
       <c r="E4" s="1">
-        <v>35.880000000000003</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="F4" s="1">
-        <v>40.11</v>
+        <v>39.94</v>
       </c>
       <c r="G4" s="1">
-        <v>35.96</v>
+        <v>36.4</v>
       </c>
       <c r="H4" s="1">
-        <v>37.03</v>
+        <v>37.31</v>
       </c>
       <c r="I4" s="1">
-        <v>42.37</v>
+        <v>43.03</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>27.35</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="1">
-        <v>39.729999999999997</v>
-      </c>
-      <c r="C5" s="1"/>
+        <v>35.950000000000003</v>
+      </c>
+      <c r="C5" s="1">
+        <v>39.36</v>
+      </c>
       <c r="D5" s="1">
-        <v>38.19</v>
+        <v>35.22</v>
       </c>
       <c r="E5" s="1">
-        <v>40.76</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>35.880000000000003</v>
+      </c>
+      <c r="F5" s="1">
+        <v>40.11</v>
+      </c>
       <c r="G5" s="1">
-        <v>39.49</v>
+        <v>35.96</v>
       </c>
       <c r="H5" s="1">
-        <v>41.48</v>
-      </c>
-      <c r="I5" s="1"/>
+        <v>37.03</v>
+      </c>
+      <c r="I5" s="1">
+        <v>42.37</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>39</v>
+        <v>27.35</v>
       </c>
       <c r="B6" s="1">
-        <v>39.85</v>
+        <v>39.729999999999997</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
-        <v>38.39</v>
+        <v>38.19</v>
       </c>
       <c r="E6" s="1">
-        <v>39.43</v>
+        <v>40.76</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1">
-        <v>39.67</v>
+        <v>39.49</v>
       </c>
       <c r="H6" s="1">
-        <v>42</v>
+        <v>41.48</v>
       </c>
       <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="2"/>
+      <c r="A7" s="1">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1">
+        <v>39.85</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>38.39</v>
+      </c>
+      <c r="E7" s="1">
+        <v>39.43</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1">
+        <v>39.67</v>
+      </c>
+      <c r="H7" s="1">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>